<commit_message>
Excel import unit tests: stats operators
</commit_message>
<xml_diff>
--- a/test/src/org/tms/io/sample3.xlsx
+++ b/test/src/org/tms/io/sample3.xlsx
@@ -4,16 +4,33 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26405"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="7940" yWindow="1780" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="17320" yWindow="1260" windowWidth="20480" windowHeight="12660" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sample 2" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
     <definedName name="Booleans">'Sample 2'!$D:$D</definedName>
-    <definedName name="Cyan">'Sample 2'!$C$5</definedName>
-    <definedName name="Subset">'Sample 2'!$B$3:$D$5</definedName>
-    <definedName name="YellowRow">'Sample 2'!$4:$4</definedName>
+    <definedName name="Count">'Sample 2'!$E$10</definedName>
+    <definedName name="Cyan">'Sample 2'!$C$9</definedName>
+    <definedName name="DevSq">'Sample 2'!$E$22</definedName>
+    <definedName name="FirstQ">'Sample 2'!$E$23</definedName>
+    <definedName name="ForthQ">'Sample 2'!$E$26</definedName>
+    <definedName name="Kurtosis">'Sample 2'!$E$21</definedName>
+    <definedName name="Max">'Sample 2'!$E$18</definedName>
+    <definedName name="Mean">'Sample 2'!$E$13</definedName>
+    <definedName name="Median">'Sample 2'!$E$14</definedName>
+    <definedName name="Min">'Sample 2'!$E$17</definedName>
+    <definedName name="Mode">'Sample 2'!$E$15</definedName>
+    <definedName name="Range">'Sample 2'!$E$11</definedName>
+    <definedName name="SecondQ">'Sample 2'!$E$24</definedName>
+    <definedName name="Skew">'Sample 2'!$E$19</definedName>
+    <definedName name="StDev">'Sample 2'!$E$16</definedName>
+    <definedName name="Subset">'Sample 2'!$B$7:$D$9</definedName>
+    <definedName name="Sum">'Sample 2'!$E$12</definedName>
+    <definedName name="SumSq">'Sample 2'!$E$20</definedName>
+    <definedName name="ThirdQ">'Sample 2'!$E$25</definedName>
+    <definedName name="YellowRow">'Sample 2'!$8:$8</definedName>
   </definedNames>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -78,7 +95,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D4" authorId="0">
+    <comment ref="D8" authorId="0">
       <text>
         <r>
           <rPr>
@@ -107,7 +124,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="28">
   <si>
     <t>Blue Row</t>
   </si>
@@ -140,6 +157,57 @@
   </si>
   <si>
     <t>Def Ghi</t>
+  </si>
+  <si>
+    <t>Sum:</t>
+  </si>
+  <si>
+    <t>Mean:</t>
+  </si>
+  <si>
+    <t>Median:</t>
+  </si>
+  <si>
+    <t>Max:</t>
+  </si>
+  <si>
+    <t>Min:</t>
+  </si>
+  <si>
+    <t>StDev:</t>
+  </si>
+  <si>
+    <t>Count:</t>
+  </si>
+  <si>
+    <t>Range:</t>
+  </si>
+  <si>
+    <t>Skew:</t>
+  </si>
+  <si>
+    <t>Sum Sq:</t>
+  </si>
+  <si>
+    <t>Mode:</t>
+  </si>
+  <si>
+    <t>Kurtosis:</t>
+  </si>
+  <si>
+    <t>Dev Sum Sq:</t>
+  </si>
+  <si>
+    <t>First Q:</t>
+  </si>
+  <si>
+    <t>Second Q:</t>
+  </si>
+  <si>
+    <t>Third Q:</t>
+  </si>
+  <si>
+    <t>Forth Q:</t>
   </si>
 </sst>
 </file>
@@ -149,7 +217,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -178,6 +246,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -193,7 +277,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -256,24 +340,57 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color theme="1"/>
-      </right>
-      <top style="thin">
-        <color theme="1"/>
-      </top>
-      <bottom style="thin">
-        <color theme="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -287,14 +404,121 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="47">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="184666" cy="261610"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5359400" y="1524000"/>
+          <a:ext cx="184666" cy="261610"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -619,7 +843,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
@@ -660,87 +884,303 @@
         <v>3</v>
       </c>
       <c r="D2" s="8" t="b">
-        <v>1</v>
+        <f>ISBLANK(B2)</f>
+        <v>0</v>
       </c>
       <c r="E2" s="9">
-        <f>'Sample 2'!$B2*3</f>
+        <f>IF(ISBLANK(B2), "", B2*3)</f>
         <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="6"/>
-      <c r="B3" s="7"/>
+      <c r="B3" s="7">
+        <v>18</v>
+      </c>
       <c r="C3" s="7"/>
-      <c r="D3" s="8"/>
+      <c r="D3" s="8" t="b">
+        <f t="shared" ref="D3:D9" si="0">ISBLANK(B3)</f>
+        <v>0</v>
+      </c>
       <c r="E3" s="9">
-        <f>'Sample 2'!$B3*3</f>
+        <f t="shared" ref="E3:E9" si="1">IF(ISBLANK(B3), "", B3*3)</f>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="6"/>
+      <c r="B4" s="7">
+        <v>17</v>
+      </c>
+      <c r="C4" s="7"/>
+      <c r="D4" s="8" t="b">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="6" t="s">
+      <c r="E4" s="9">
+        <f t="shared" si="1"/>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="6"/>
+      <c r="B5" s="7">
+        <v>11</v>
+      </c>
+      <c r="C5" s="7"/>
+      <c r="D5" s="8" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E5" s="9">
+        <f t="shared" si="1"/>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="6"/>
+      <c r="B6" s="7">
+        <v>12</v>
+      </c>
+      <c r="C6" s="7"/>
+      <c r="D6" s="8" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E6" s="9">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="6"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="8" t="b">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7" t="s">
+      <c r="E7" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="8" t="b">
+      <c r="D8" s="8" t="b">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="E4" s="9">
-        <f>'Sample 2'!$B4*3</f>
+      <c r="E8" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="11">
+        <v>17.649999999999999</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="12" t="b">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="11">
-        <v>17.649999999999999</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="E5" s="13">
-        <f>'Sample 2'!$B5*3</f>
+      <c r="E9" s="9">
+        <f t="shared" si="1"/>
         <v>52.949999999999996</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
-      <c r="B6" s="1">
-        <f>SUM(B2:B5)</f>
-        <v>29.65</v>
-      </c>
-      <c r="E6">
-        <f>SUM(E2:E5)</f>
-        <v>88.949999999999989</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="B7" s="1">
-        <f>AVERAGE(B2:B5)</f>
-        <v>14.824999999999999</v>
-      </c>
-      <c r="E7">
-        <f>AVERAGE(E2:E5)</f>
-        <v>22.237499999999997</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="E8">
-        <f>MEDIAN(E2:E5)</f>
+    <row r="10" spans="1:5">
+      <c r="A10" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="15">
+        <f>COUNT(B2:B9)</f>
+        <v>6</v>
+      </c>
+      <c r="C10" s="15"/>
+      <c r="D10" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="14">
+        <f>COUNT(E2:E9)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="1">
+        <f>SUM(B2:B9)</f>
+        <v>87.65</v>
+      </c>
+      <c r="D11" s="16" t="s">
         <v>18</v>
+      </c>
+      <c r="E11" s="14">
+        <f>MAX(E2:E9) - MIN(E2:E9)</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="1">
+        <f>AVERAGE(B2:B9)</f>
+        <v>14.608333333333334</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12">
+        <f>SUM(E2:E9)</f>
+        <v>262.95</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="D13" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="E13">
+        <f>AVERAGE(E2:E9)</f>
+        <v>43.824999999999996</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="D14" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14">
+        <f>MEDIAN(E2:E9)</f>
+        <v>43.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="D15" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="E15">
+        <f>MODE(E2:E9)</f>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="D16" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="E16">
+        <f>STDEV(E2:E9)</f>
+        <v>9.7766942265778045</v>
+      </c>
+    </row>
+    <row r="17" spans="4:5">
+      <c r="D17" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="E17">
+        <f>MIN(E2:E9)</f>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="4:5">
+      <c r="D18" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="E18">
+        <f>MAX(E2:E9)</f>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="19" spans="4:5">
+      <c r="D19" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="E19">
+        <f>SKEW(E2:E9)</f>
+        <v>-1.4171252356635732E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="4:5">
+      <c r="D20" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="E20">
+        <f>SUMSQ(E2:E9)</f>
+        <v>12001.702499999999</v>
+      </c>
+    </row>
+    <row r="21" spans="4:5">
+      <c r="D21" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="E21">
+        <f>KURT(E2:E9)</f>
+        <v>-3.0679317993382256</v>
+      </c>
+    </row>
+    <row r="22" spans="4:5">
+      <c r="D22" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="E22">
+        <f>DEVSQ(E2:E9)</f>
+        <v>477.91874999999993</v>
+      </c>
+    </row>
+    <row r="23" spans="4:5">
+      <c r="D23" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="E23">
+        <f>QUARTILE(E2:E9, 1)</f>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="24" spans="4:5">
+      <c r="D24" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="E24">
+        <f>QUARTILE(E2:E9, 2)</f>
+        <v>43.5</v>
+      </c>
+    </row>
+    <row r="25" spans="4:5">
+      <c r="D25" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="E25">
+        <f>QUARTILE(E2:E9, 3)</f>
+        <v>52.462499999999999</v>
+      </c>
+    </row>
+    <row r="26" spans="4:5">
+      <c r="D26" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="E26">
+        <f>QUARTILE(E2:E9, 4)</f>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <legacyDrawing r:id="rId1"/>
+  <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Checkpoint of Excel Import; Added more functions Completed Stats Unit Test Added String function Unit Tests
</commit_message>
<xml_diff>
--- a/test/src/org/tms/io/sample3.xlsx
+++ b/test/src/org/tms/io/sample3.xlsx
@@ -4,33 +4,37 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26405"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="17320" yWindow="1260" windowWidth="20480" windowHeight="12660" tabRatio="500"/>
+    <workbookView xWindow="7800" yWindow="320" windowWidth="14440" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sample 2" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="Booleans">'Sample 2'!$D:$D</definedName>
     <definedName name="Count">'Sample 2'!$E$10</definedName>
     <definedName name="Cyan">'Sample 2'!$C$9</definedName>
-    <definedName name="DevSq">'Sample 2'!$E$22</definedName>
-    <definedName name="FirstQ">'Sample 2'!$E$23</definedName>
-    <definedName name="ForthQ">'Sample 2'!$E$26</definedName>
-    <definedName name="Kurtosis">'Sample 2'!$E$21</definedName>
-    <definedName name="Max">'Sample 2'!$E$18</definedName>
+    <definedName name="DevSq">'Sample 2'!$E$23</definedName>
+    <definedName name="FirstQ">'Sample 2'!$E$24</definedName>
+    <definedName name="ForthQ">'Sample 2'!$E$27</definedName>
+    <definedName name="Kurtosis">'Sample 2'!$E$22</definedName>
+    <definedName name="LOWERCASE">'Sample 2'!$C$15</definedName>
+    <definedName name="Max">'Sample 2'!$E$19</definedName>
     <definedName name="Mean">'Sample 2'!$E$13</definedName>
     <definedName name="Median">'Sample 2'!$E$14</definedName>
-    <definedName name="Min">'Sample 2'!$E$17</definedName>
+    <definedName name="Min">'Sample 2'!$E$18</definedName>
     <definedName name="Mode">'Sample 2'!$E$15</definedName>
+    <definedName name="Pi">'Sample 2'!$B$14</definedName>
     <definedName name="Range">'Sample 2'!$E$11</definedName>
-    <definedName name="SecondQ">'Sample 2'!$E$24</definedName>
-    <definedName name="Skew">'Sample 2'!$E$19</definedName>
-    <definedName name="StDev">'Sample 2'!$E$16</definedName>
-    <definedName name="Subset">'Sample 2'!$B$7:$D$9</definedName>
+    <definedName name="SecondQ">'Sample 2'!$E$25</definedName>
+    <definedName name="Skew">'Sample 2'!$E$20</definedName>
+    <definedName name="StDev.S">'Sample 2'!$E$16</definedName>
     <definedName name="Sum">'Sample 2'!$E$12</definedName>
-    <definedName name="SumSq">'Sample 2'!$E$20</definedName>
-    <definedName name="ThirdQ">'Sample 2'!$E$25</definedName>
+    <definedName name="SumSq">'Sample 2'!$E$21</definedName>
+    <definedName name="ThirdQ">'Sample 2'!$E$26</definedName>
+    <definedName name="UPPERCASE">'Sample 2'!$C$14</definedName>
+    <definedName name="Var.S">'Sample 2'!$E$17</definedName>
+    <definedName name="YellowLen">'Sample 2'!$C$16</definedName>
     <definedName name="YellowRow">'Sample 2'!$8:$8</definedName>
+    <definedName name="YellowTrim">'Sample 2'!$C$17</definedName>
   </definedNames>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -124,7 +128,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="32">
   <si>
     <t>Blue Row</t>
   </si>
@@ -174,9 +178,6 @@
     <t>Min:</t>
   </si>
   <si>
-    <t>StDev:</t>
-  </si>
-  <si>
     <t>Count:</t>
   </si>
   <si>
@@ -208,6 +209,21 @@
   </si>
   <si>
     <t>Forth Q:</t>
+  </si>
+  <si>
+    <t>StDev (S):</t>
+  </si>
+  <si>
+    <t>Var (S)</t>
+  </si>
+  <si>
+    <t>Pi:</t>
+  </si>
+  <si>
+    <t>Yellow Len:</t>
+  </si>
+  <si>
+    <t>Trimmed:</t>
   </si>
 </sst>
 </file>
@@ -217,7 +233,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -261,6 +277,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color indexed="206"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -341,7 +363,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="47">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -389,8 +411,10 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -412,8 +436,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="47">
+  <cellStyles count="49">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -437,6 +465,7 @@
     <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -460,6 +489,7 @@
     <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -843,7 +873,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
@@ -1003,7 +1033,7 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B10" s="15">
         <f>COUNT(B2:B9)</f>
@@ -1011,7 +1041,7 @@
       </c>
       <c r="C10" s="15"/>
       <c r="D10" s="16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E10" s="14">
         <f>COUNT(E2:E9)</f>
@@ -1027,7 +1057,7 @@
         <v>87.65</v>
       </c>
       <c r="D11" s="16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E11" s="14">
         <f>MAX(E2:E9) - MIN(E2:E9)</f>
@@ -1060,6 +1090,17 @@
       </c>
     </row>
     <row r="14" spans="1:5">
+      <c r="A14" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" s="1">
+        <f>PI()</f>
+        <v>3.1415926535897931</v>
+      </c>
+      <c r="C14" t="str">
+        <f>UPPER(C8)</f>
+        <v>YELLOW</v>
+      </c>
       <c r="D14" s="13" t="s">
         <v>13</v>
       </c>
@@ -1069,8 +1110,13 @@
       </c>
     </row>
     <row r="15" spans="1:5">
+      <c r="B15" s="18"/>
+      <c r="C15" t="str">
+        <f>LOWER(Cyan)</f>
+        <v>cyan</v>
+      </c>
       <c r="D15" s="13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E15">
         <f>MODE(E2:E9)</f>
@@ -1078,100 +1124,123 @@
       </c>
     </row>
     <row r="16" spans="1:5">
+      <c r="B16" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16">
+        <f>LEN(C8)</f>
+        <v>6</v>
+      </c>
       <c r="D16" s="13" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="E16">
         <f>STDEV(E2:E9)</f>
         <v>9.7766942265778045</v>
       </c>
     </row>
-    <row r="17" spans="4:5">
+    <row r="17" spans="2:5">
+      <c r="B17" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17" t="str">
+        <f>TRIM(CONCATENATE(C8, "   "))</f>
+        <v>Yellow</v>
+      </c>
       <c r="D17" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="E17">
+        <f>VAR(E2:E9)</f>
+        <v>95.583749999999782</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5">
+      <c r="D18" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="E17">
+      <c r="E18">
         <f>MIN(E2:E9)</f>
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="4:5">
-      <c r="D18" s="13" t="s">
+    <row r="19" spans="2:5">
+      <c r="D19" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="E18">
+      <c r="E19">
         <f>MAX(E2:E9)</f>
         <v>54</v>
       </c>
     </row>
-    <row r="19" spans="4:5">
-      <c r="D19" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="E19">
+    <row r="20" spans="2:5">
+      <c r="D20" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="E20">
         <f>SKEW(E2:E9)</f>
         <v>-1.4171252356635732E-2</v>
       </c>
     </row>
-    <row r="20" spans="4:5">
-      <c r="D20" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="E20">
+    <row r="21" spans="2:5">
+      <c r="D21" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="E21">
         <f>SUMSQ(E2:E9)</f>
         <v>12001.702499999999</v>
       </c>
     </row>
-    <row r="21" spans="4:5">
-      <c r="D21" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="E21">
+    <row r="22" spans="2:5">
+      <c r="D22" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="E22">
         <f>KURT(E2:E9)</f>
         <v>-3.0679317993382256</v>
       </c>
     </row>
-    <row r="22" spans="4:5">
-      <c r="D22" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="E22">
+    <row r="23" spans="2:5">
+      <c r="D23" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="E23">
         <f>DEVSQ(E2:E9)</f>
         <v>477.91874999999993</v>
       </c>
     </row>
-    <row r="23" spans="4:5">
-      <c r="D23" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="E23">
+    <row r="24" spans="2:5">
+      <c r="D24" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="E24">
         <f>QUARTILE(E2:E9, 1)</f>
         <v>36</v>
       </c>
     </row>
-    <row r="24" spans="4:5">
-      <c r="D24" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="E24">
+    <row r="25" spans="2:5">
+      <c r="D25" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="E25">
         <f>QUARTILE(E2:E9, 2)</f>
         <v>43.5</v>
       </c>
     </row>
-    <row r="25" spans="4:5">
-      <c r="D25" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="E25">
+    <row r="26" spans="2:5">
+      <c r="D26" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="E26">
         <f>QUARTILE(E2:E9, 3)</f>
         <v>52.462499999999999</v>
       </c>
     </row>
-    <row r="26" spans="4:5">
-      <c r="D26" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="E26">
+    <row r="27" spans="2:5">
+      <c r="D27" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="E27">
         <f>QUARTILE(E2:E9, 4)</f>
         <v>54</v>
       </c>

</xml_diff>

<commit_message>
Checkpoint Excel Import; Added more string functions for Excel parity Added unit tests for String functions
</commit_message>
<xml_diff>
--- a/test/src/org/tms/io/sample3.xlsx
+++ b/test/src/org/tms/io/sample3.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26405"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="7800" yWindow="320" windowWidth="14440" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="17960" yWindow="0" windowWidth="18260" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sample 2" sheetId="1" r:id="rId1"/>
@@ -15,15 +15,26 @@
     <definedName name="DevSq">'Sample 2'!$E$23</definedName>
     <definedName name="FirstQ">'Sample 2'!$E$24</definedName>
     <definedName name="ForthQ">'Sample 2'!$E$27</definedName>
+    <definedName name="IsErrorVal">'Sample 2'!$C$24</definedName>
+    <definedName name="IsErrVal">'Sample 2'!$C$23</definedName>
+    <definedName name="IsLogicalVal">'Sample 2'!$C$22</definedName>
+    <definedName name="IsNumberVal">'Sample 2'!$C$21</definedName>
+    <definedName name="IsSameValStr">'Sample 2'!$C$25</definedName>
+    <definedName name="IsTextVal">'Sample 2'!$C$20</definedName>
     <definedName name="Kurtosis">'Sample 2'!$E$22</definedName>
+    <definedName name="LeftVal">'Sample 2'!$C$27</definedName>
     <definedName name="LOWERCASE">'Sample 2'!$C$15</definedName>
+    <definedName name="ManyCyan">'Sample 2'!$C$19</definedName>
     <definedName name="Max">'Sample 2'!$E$19</definedName>
     <definedName name="Mean">'Sample 2'!$E$13</definedName>
     <definedName name="Median">'Sample 2'!$E$14</definedName>
+    <definedName name="MidVal">'Sample 2'!$C$29</definedName>
     <definedName name="Min">'Sample 2'!$E$18</definedName>
     <definedName name="Mode">'Sample 2'!$E$15</definedName>
-    <definedName name="Pi">'Sample 2'!$B$14</definedName>
+    <definedName name="PiVal">'Sample 2'!$C$13</definedName>
+    <definedName name="PiValStr">'Sample 2'!$C$26</definedName>
     <definedName name="Range">'Sample 2'!$E$11</definedName>
+    <definedName name="RightVal">'Sample 2'!$C$28</definedName>
     <definedName name="SecondQ">'Sample 2'!$E$25</definedName>
     <definedName name="Skew">'Sample 2'!$E$20</definedName>
     <definedName name="StDev.S">'Sample 2'!$E$16</definedName>
@@ -32,9 +43,11 @@
     <definedName name="ThirdQ">'Sample 2'!$E$26</definedName>
     <definedName name="UPPERCASE">'Sample 2'!$C$14</definedName>
     <definedName name="Var.S">'Sample 2'!$E$17</definedName>
+    <definedName name="YellowCyan">'Sample 2'!$C$18</definedName>
     <definedName name="YellowLen">'Sample 2'!$C$16</definedName>
     <definedName name="YellowRow">'Sample 2'!$8:$8</definedName>
     <definedName name="YellowTrim">'Sample 2'!$C$17</definedName>
+    <definedName name="YeyanVal">'Sample 2'!$C$30</definedName>
   </definedNames>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -128,7 +141,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="47">
   <si>
     <t>Blue Row</t>
   </si>
@@ -224,6 +237,51 @@
   </si>
   <si>
     <t>Trimmed:</t>
+  </si>
+  <si>
+    <t>Lowercase:</t>
+  </si>
+  <si>
+    <t>Uppercase:</t>
+  </si>
+  <si>
+    <t>Concatination:</t>
+  </si>
+  <si>
+    <t>String Mult:</t>
+  </si>
+  <si>
+    <t>Is Text:</t>
+  </si>
+  <si>
+    <t>Is Number:</t>
+  </si>
+  <si>
+    <t>Is Logical:</t>
+  </si>
+  <si>
+    <t>Is Error:</t>
+  </si>
+  <si>
+    <t>Is Err:</t>
+  </si>
+  <si>
+    <t>Is Same (Text):</t>
+  </si>
+  <si>
+    <t>Value:</t>
+  </si>
+  <si>
+    <t>Left Str:</t>
+  </si>
+  <si>
+    <t>Right Str:</t>
+  </si>
+  <si>
+    <t>Mid Str:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Str Func: </t>
   </si>
 </sst>
 </file>
@@ -363,7 +421,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -413,8 +471,20 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -439,9 +509,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="61">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -466,6 +541,12 @@
     <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -490,6 +571,12 @@
     <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -873,7 +960,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E27"/>
+  <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
@@ -882,7 +969,8 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="2" max="2" width="10.83203125" style="1"/>
+    <col min="2" max="2" width="14" style="1" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" customWidth="1"/>
     <col min="4" max="4" width="18" customWidth="1"/>
   </cols>
   <sheetData>
@@ -985,7 +1073,10 @@
     <row r="7" spans="1:5">
       <c r="A7" s="6"/>
       <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
+      <c r="C7" s="7" t="e">
+        <f>1/0</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="D7" s="8" t="b">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -1081,6 +1172,13 @@
       </c>
     </row>
     <row r="13" spans="1:5">
+      <c r="B13" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13">
+        <f>PI()</f>
+        <v>3.1415926535897931</v>
+      </c>
       <c r="D13" s="13" t="s">
         <v>12</v>
       </c>
@@ -1090,12 +1188,9 @@
       </c>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="B14" s="1">
-        <f>PI()</f>
-        <v>3.1415926535897931</v>
+      <c r="A14" s="17"/>
+      <c r="B14" s="18" t="s">
+        <v>33</v>
       </c>
       <c r="C14" t="str">
         <f>UPPER(C8)</f>
@@ -1110,7 +1205,9 @@
       </c>
     </row>
     <row r="15" spans="1:5">
-      <c r="B15" s="18"/>
+      <c r="B15" s="19" t="s">
+        <v>32</v>
+      </c>
       <c r="C15" t="str">
         <f>LOWER(Cyan)</f>
         <v>cyan</v>
@@ -1124,7 +1221,7 @@
       </c>
     </row>
     <row r="16" spans="1:5">
-      <c r="B16" s="1" t="s">
+      <c r="B16" s="18" t="s">
         <v>30</v>
       </c>
       <c r="C16">
@@ -1140,7 +1237,7 @@
       </c>
     </row>
     <row r="17" spans="2:5">
-      <c r="B17" s="1" t="s">
+      <c r="B17" s="18" t="s">
         <v>31</v>
       </c>
       <c r="C17" t="str">
@@ -1156,6 +1253,13 @@
       </c>
     </row>
     <row r="18" spans="2:5">
+      <c r="B18" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="C18" t="str">
+        <f>C8&amp;Cyan&amp;C2</f>
+        <v>YellowCyanBlue</v>
+      </c>
       <c r="D18" s="13" t="s">
         <v>15</v>
       </c>
@@ -1165,6 +1269,13 @@
       </c>
     </row>
     <row r="19" spans="2:5">
+      <c r="B19" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="C19" t="str">
+        <f>REPT(Cyan, 3)</f>
+        <v>CyanCyanCyan</v>
+      </c>
       <c r="D19" s="13" t="s">
         <v>14</v>
       </c>
@@ -1174,6 +1285,13 @@
       </c>
     </row>
     <row r="20" spans="2:5">
+      <c r="B20" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="C20" t="b">
+        <f>ISTEXT(C8)</f>
+        <v>1</v>
+      </c>
       <c r="D20" s="13" t="s">
         <v>18</v>
       </c>
@@ -1183,6 +1301,13 @@
       </c>
     </row>
     <row r="21" spans="2:5">
+      <c r="B21" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="C21" t="b">
+        <f>ISNUMBER(C8)</f>
+        <v>0</v>
+      </c>
       <c r="D21" s="13" t="s">
         <v>19</v>
       </c>
@@ -1192,6 +1317,13 @@
       </c>
     </row>
     <row r="22" spans="2:5">
+      <c r="B22" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="C22" t="b">
+        <f>ISLOGICAL(IsNumberVal)</f>
+        <v>1</v>
+      </c>
       <c r="D22" s="13" t="s">
         <v>21</v>
       </c>
@@ -1201,6 +1333,13 @@
       </c>
     </row>
     <row r="23" spans="2:5">
+      <c r="B23" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="C23" t="b">
+        <f>ISERR(C7)</f>
+        <v>1</v>
+      </c>
       <c r="D23" s="13" t="s">
         <v>22</v>
       </c>
@@ -1210,6 +1349,13 @@
       </c>
     </row>
     <row r="24" spans="2:5">
+      <c r="B24" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="C24" t="b">
+        <f>ISERROR(C7)</f>
+        <v>1</v>
+      </c>
       <c r="D24" s="13" t="s">
         <v>23</v>
       </c>
@@ -1219,6 +1365,13 @@
       </c>
     </row>
     <row r="25" spans="2:5">
+      <c r="B25" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="C25" t="b">
+        <f>EXACT(C8,Cyan)</f>
+        <v>0</v>
+      </c>
       <c r="D25" s="13" t="s">
         <v>24</v>
       </c>
@@ -1228,6 +1381,13 @@
       </c>
     </row>
     <row r="26" spans="2:5">
+      <c r="B26" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="C26">
+        <f>VALUE("3.141592654")</f>
+        <v>3.1415926540000001</v>
+      </c>
       <c r="D26" s="13" t="s">
         <v>25</v>
       </c>
@@ -1237,12 +1397,46 @@
       </c>
     </row>
     <row r="27" spans="2:5">
+      <c r="B27" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="C27" t="str">
+        <f xml:space="preserve"> LEFT(C8,4)</f>
+        <v>Yell</v>
+      </c>
       <c r="D27" s="13" t="s">
         <v>26</v>
       </c>
       <c r="E27">
         <f>QUARTILE(E2:E9, 4)</f>
         <v>54</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5">
+      <c r="B28" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="C28" t="str">
+        <f>RIGHT(C8,3)</f>
+        <v>low</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5">
+      <c r="B29" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="C29" t="str">
+        <f>MID(C8,2,3)</f>
+        <v>ell</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5">
+      <c r="B30" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="C30" t="str">
+        <f>LEFT(C8,2) &amp; RIGHT(Cyan,3)</f>
+        <v>Yeyan</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Checkpoint of Excel Importer Removed java-like mod operator (%) Implemented % operator (for Excel) Regiggered unit tests accordingly
</commit_message>
<xml_diff>
--- a/test/src/org/tms/io/sample3.xlsx
+++ b/test/src/org/tms/io/sample3.xlsx
@@ -4,15 +4,18 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26405"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="17960" yWindow="0" windowWidth="18260" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11920" windowHeight="13900" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sample 2" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
+    <definedName name="BasicMathVal">'Sample 2'!$C$6</definedName>
+    <definedName name="ComplexPowerVal">'Sample 2'!$C$5</definedName>
     <definedName name="Count">'Sample 2'!$E$10</definedName>
     <definedName name="Cyan">'Sample 2'!$C$9</definedName>
     <definedName name="DevSq">'Sample 2'!$E$23</definedName>
+    <definedName name="FactorialVal">'Sample 2'!$C$10</definedName>
     <definedName name="FirstQ">'Sample 2'!$E$24</definedName>
     <definedName name="ForthQ">'Sample 2'!$E$27</definedName>
     <definedName name="IsErrorVal">'Sample 2'!$C$24</definedName>
@@ -31,8 +34,10 @@
     <definedName name="MidVal">'Sample 2'!$C$29</definedName>
     <definedName name="Min">'Sample 2'!$E$18</definedName>
     <definedName name="Mode">'Sample 2'!$E$15</definedName>
+    <definedName name="PercentageVal">'Sample 2'!$C$3</definedName>
     <definedName name="PiVal">'Sample 2'!$C$13</definedName>
     <definedName name="PiValStr">'Sample 2'!$C$26</definedName>
+    <definedName name="PowerVal">'Sample 2'!$C$4</definedName>
     <definedName name="Range">'Sample 2'!$E$11</definedName>
     <definedName name="RightVal">'Sample 2'!$C$28</definedName>
     <definedName name="SecondQ">'Sample 2'!$E$25</definedName>
@@ -1015,7 +1020,10 @@
       <c r="B3" s="7">
         <v>18</v>
       </c>
-      <c r="C3" s="7"/>
+      <c r="C3" s="7">
+        <f>BasicMathVal*50%</f>
+        <v>2</v>
+      </c>
       <c r="D3" s="8" t="b">
         <f t="shared" ref="D3:D9" si="0">ISBLANK(B3)</f>
         <v>0</v>
@@ -1030,7 +1038,10 @@
       <c r="B4" s="7">
         <v>17</v>
       </c>
-      <c r="C4" s="7"/>
+      <c r="C4" s="7">
+        <f>POWER(3,4)</f>
+        <v>81</v>
+      </c>
       <c r="D4" s="8" t="b">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1045,7 +1056,10 @@
       <c r="B5" s="7">
         <v>11</v>
       </c>
-      <c r="C5" s="7"/>
+      <c r="C5" s="7">
+        <f>POWER((1+2-3*4/6+MOD(5,2))^2,3)</f>
+        <v>64</v>
+      </c>
       <c r="D5" s="8" t="b">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1060,7 +1074,10 @@
       <c r="B6" s="7">
         <v>12</v>
       </c>
-      <c r="C6" s="7"/>
+      <c r="C6" s="7">
+        <f>(1+2-3*4/6+MOD(5,2))^2</f>
+        <v>4</v>
+      </c>
       <c r="D6" s="8" t="b">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1130,7 +1147,10 @@
         <f>COUNT(B2:B9)</f>
         <v>6</v>
       </c>
-      <c r="C10" s="15"/>
+      <c r="C10" s="15">
+        <f>FACT(BasicMathVal)</f>
+        <v>24</v>
+      </c>
       <c r="D10" s="16" t="s">
         <v>16</v>
       </c>

</xml_diff>